<commit_message>
feat:add new migration, fix template and new information on discrepancy statistics
</commit_message>
<xml_diff>
--- a/storage/app/templates/worksheet_template.xlsx
+++ b/storage/app/templates/worksheet_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ngulik\kerja\TMMIN\inventory-checkup\storage\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468535ED-B5F1-4352-AC55-C34AB29A3235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC4148B-3236-4887-8D4D-A0A6E8A1240E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{99ADF681-7D44-47EE-A388-433CE60AD921}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="40">
   <si>
     <t>WORKSHEET DATA</t>
   </si>
@@ -169,12 +169,33 @@
   <si>
     <t>[items.actual_qty]</t>
   </si>
+  <si>
+    <t>Checked</t>
+  </si>
+  <si>
+    <t>Counted</t>
+  </si>
+  <si>
+    <t>PIC Input</t>
+  </si>
+  <si>
+    <t>PIC Check</t>
+  </si>
+  <si>
+    <t>[pic_input]</t>
+  </si>
+  <si>
+    <t>[group_leader]</t>
+  </si>
+  <si>
+    <t>[pic_name]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,8 +269,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +294,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="13"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -475,6 +522,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -493,11 +546,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -565,6 +628,49 @@
           <a:tailEnd/>
         </a:ln>
       </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="2400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>17:30 WIB</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -629,13 +735,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2491740</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -652,7 +758,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2133600" y="3108960"/>
+          <a:off x="2133600" y="3131820"/>
           <a:ext cx="2148840" cy="441960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -670,6 +776,16 @@
           <a:tailEnd/>
         </a:ln>
       </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400"/>
+            <a:t>16:00 WIB</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -727,144 +843,6 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3002280</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>929640</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{210BF107-F973-4FC8-BF35-E21558B746BE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4792980" y="175260"/>
-          <a:ext cx="1920240" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>960120</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>891540</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30527D18-9799-4911-80F5-E909BB41FCC8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6743700" y="175260"/>
-          <a:ext cx="1874520" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
@@ -1559,8 +1537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABECC8FE-D70C-47E6-B52B-70D95AF9CDE8}">
   <dimension ref="A1:I336"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A322" sqref="A245:XFD322"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1569,9 +1547,9 @@
     <col min="2" max="2" width="7.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
     <col min="4" max="4" width="49.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="2"/>
-    <col min="6" max="6" width="17.88671875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="2" customWidth="1"/>
     <col min="8" max="8" width="13.44140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="10" max="250" width="9.109375" style="1" customWidth="1"/>
@@ -2536,36 +2514,75 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
+      <c r="E2" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="13.8" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:8" ht="13.8" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:8" ht="13.8" x14ac:dyDescent="0.25"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+    </row>
+    <row r="4" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+    </row>
+    <row r="5" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+    </row>
+    <row r="6" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="E6" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="7" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="13.8" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -6586,136 +6603,141 @@
       <c r="H322" s="15"/>
     </row>
     <row r="323" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B323" s="27"/>
-      <c r="C323" s="27"/>
-      <c r="D323" s="28"/>
-      <c r="E323" s="27"/>
-      <c r="F323" s="27"/>
-      <c r="G323" s="27"/>
-      <c r="H323" s="27"/>
+      <c r="B323" s="21"/>
+      <c r="C323" s="21"/>
+      <c r="D323" s="22"/>
+      <c r="E323" s="21"/>
+      <c r="F323" s="21"/>
+      <c r="G323" s="21"/>
+      <c r="H323" s="21"/>
     </row>
     <row r="324" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B324" s="27"/>
-      <c r="C324" s="27"/>
-      <c r="D324" s="28"/>
-      <c r="E324" s="27"/>
-      <c r="F324" s="27"/>
-      <c r="G324" s="27"/>
-      <c r="H324" s="27"/>
+      <c r="B324" s="21"/>
+      <c r="C324" s="21"/>
+      <c r="D324" s="22"/>
+      <c r="E324" s="21"/>
+      <c r="F324" s="21"/>
+      <c r="G324" s="21"/>
+      <c r="H324" s="21"/>
     </row>
     <row r="325" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B325" s="27"/>
-      <c r="C325" s="27"/>
-      <c r="D325" s="28"/>
-      <c r="E325" s="27"/>
-      <c r="F325" s="27"/>
-      <c r="G325" s="27"/>
-      <c r="H325" s="27"/>
+      <c r="B325" s="21"/>
+      <c r="C325" s="21"/>
+      <c r="D325" s="22"/>
+      <c r="E325" s="21"/>
+      <c r="F325" s="21"/>
+      <c r="G325" s="21"/>
+      <c r="H325" s="21"/>
     </row>
     <row r="326" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B326" s="27"/>
-      <c r="C326" s="27"/>
-      <c r="D326" s="28"/>
-      <c r="E326" s="27"/>
-      <c r="F326" s="27"/>
-      <c r="G326" s="27"/>
-      <c r="H326" s="27"/>
+      <c r="B326" s="21"/>
+      <c r="C326" s="21"/>
+      <c r="D326" s="22"/>
+      <c r="E326" s="21"/>
+      <c r="F326" s="21"/>
+      <c r="G326" s="21"/>
+      <c r="H326" s="21"/>
     </row>
     <row r="327" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B327" s="27"/>
-      <c r="C327" s="27"/>
-      <c r="D327" s="28"/>
-      <c r="E327" s="27"/>
-      <c r="F327" s="27"/>
-      <c r="G327" s="27"/>
-      <c r="H327" s="27"/>
+      <c r="B327" s="21"/>
+      <c r="C327" s="21"/>
+      <c r="D327" s="22"/>
+      <c r="E327" s="21"/>
+      <c r="F327" s="21"/>
+      <c r="G327" s="21"/>
+      <c r="H327" s="21"/>
     </row>
     <row r="328" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B328" s="27"/>
-      <c r="C328" s="27"/>
-      <c r="D328" s="28"/>
-      <c r="E328" s="27"/>
-      <c r="F328" s="27"/>
-      <c r="G328" s="27"/>
-      <c r="H328" s="27"/>
+      <c r="B328" s="21"/>
+      <c r="C328" s="21"/>
+      <c r="D328" s="22"/>
+      <c r="E328" s="21"/>
+      <c r="F328" s="21"/>
+      <c r="G328" s="21"/>
+      <c r="H328" s="21"/>
     </row>
     <row r="329" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B329" s="27"/>
-      <c r="C329" s="27"/>
-      <c r="D329" s="28"/>
-      <c r="E329" s="27"/>
-      <c r="F329" s="27"/>
-      <c r="G329" s="27"/>
-      <c r="H329" s="27"/>
+      <c r="B329" s="21"/>
+      <c r="C329" s="21"/>
+      <c r="D329" s="22"/>
+      <c r="E329" s="21"/>
+      <c r="F329" s="21"/>
+      <c r="G329" s="21"/>
+      <c r="H329" s="21"/>
     </row>
     <row r="330" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B330" s="27"/>
-      <c r="C330" s="27"/>
-      <c r="D330" s="28"/>
-      <c r="E330" s="27"/>
-      <c r="F330" s="27"/>
-      <c r="G330" s="27"/>
-      <c r="H330" s="27"/>
+      <c r="B330" s="21"/>
+      <c r="C330" s="21"/>
+      <c r="D330" s="22"/>
+      <c r="E330" s="21"/>
+      <c r="F330" s="21"/>
+      <c r="G330" s="21"/>
+      <c r="H330" s="21"/>
     </row>
     <row r="331" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B331" s="27"/>
-      <c r="C331" s="27"/>
-      <c r="D331" s="28"/>
-      <c r="E331" s="27"/>
-      <c r="F331" s="27"/>
-      <c r="G331" s="27"/>
-      <c r="H331" s="27"/>
+      <c r="B331" s="21"/>
+      <c r="C331" s="21"/>
+      <c r="D331" s="22"/>
+      <c r="E331" s="21"/>
+      <c r="F331" s="21"/>
+      <c r="G331" s="21"/>
+      <c r="H331" s="21"/>
     </row>
     <row r="332" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B332" s="27"/>
-      <c r="C332" s="27"/>
-      <c r="D332" s="28"/>
-      <c r="E332" s="27"/>
-      <c r="F332" s="27"/>
-      <c r="G332" s="27"/>
-      <c r="H332" s="27"/>
+      <c r="B332" s="21"/>
+      <c r="C332" s="21"/>
+      <c r="D332" s="22"/>
+      <c r="E332" s="21"/>
+      <c r="F332" s="21"/>
+      <c r="G332" s="21"/>
+      <c r="H332" s="21"/>
     </row>
     <row r="333" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B333" s="27"/>
-      <c r="C333" s="27"/>
-      <c r="D333" s="28"/>
-      <c r="E333" s="27"/>
-      <c r="F333" s="27"/>
-      <c r="G333" s="27"/>
-      <c r="H333" s="27"/>
+      <c r="B333" s="21"/>
+      <c r="C333" s="21"/>
+      <c r="D333" s="22"/>
+      <c r="E333" s="21"/>
+      <c r="F333" s="21"/>
+      <c r="G333" s="21"/>
+      <c r="H333" s="21"/>
     </row>
     <row r="334" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B334" s="27"/>
-      <c r="C334" s="27"/>
-      <c r="D334" s="28"/>
-      <c r="E334" s="27"/>
-      <c r="F334" s="27"/>
-      <c r="G334" s="27"/>
-      <c r="H334" s="27"/>
+      <c r="B334" s="21"/>
+      <c r="C334" s="21"/>
+      <c r="D334" s="22"/>
+      <c r="E334" s="21"/>
+      <c r="F334" s="21"/>
+      <c r="G334" s="21"/>
+      <c r="H334" s="21"/>
     </row>
     <row r="335" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B335" s="27"/>
-      <c r="C335" s="27"/>
-      <c r="D335" s="28"/>
-      <c r="E335" s="27"/>
-      <c r="F335" s="27"/>
-      <c r="G335" s="27"/>
-      <c r="H335" s="27"/>
+      <c r="B335" s="21"/>
+      <c r="C335" s="21"/>
+      <c r="D335" s="22"/>
+      <c r="E335" s="21"/>
+      <c r="F335" s="21"/>
+      <c r="G335" s="21"/>
+      <c r="H335" s="21"/>
     </row>
     <row r="336" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B336" s="27"/>
-      <c r="C336" s="27"/>
-      <c r="D336" s="28"/>
-      <c r="E336" s="27"/>
-      <c r="F336" s="27"/>
-      <c r="G336" s="27"/>
-      <c r="H336" s="27"/>
+      <c r="B336" s="21"/>
+      <c r="C336" s="21"/>
+      <c r="D336" s="22"/>
+      <c r="E336" s="21"/>
+      <c r="F336" s="21"/>
+      <c r="G336" s="21"/>
+      <c r="H336" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="B8:H9"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="H3:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat:add fiscal year on PID List
</commit_message>
<xml_diff>
--- a/storage/app/templates/worksheet_template.xlsx
+++ b/storage/app/templates/worksheet_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ngulik\kerja\TMMIN\inventory-checkup\storage\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C13949-01CF-4F33-83E3-9FF5886A17B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E033F1-C3EC-46C5-B274-0A70ED5DC2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{99ADF681-7D44-47EE-A388-433CE60AD921}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="42">
   <si>
     <t>WORKSHEET DATA</t>
   </si>
@@ -119,13 +119,7 @@
     <t xml:space="preserve">     JAM MULAI</t>
   </si>
   <si>
-    <t xml:space="preserve">                                                                                     JAM SELESAI</t>
-  </si>
-  <si>
     <t xml:space="preserve">     MENGHITUNG :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                     MENGHITUNG :</t>
   </si>
   <si>
     <t>NO.</t>
@@ -190,12 +184,24 @@
   <si>
     <t>[pic_name]</t>
   </si>
+  <si>
+    <t>16:30 WIB</t>
+  </si>
+  <si>
+    <t>JAM SELESAI</t>
+  </si>
+  <si>
+    <t>MENGHITUNG :</t>
+  </si>
+  <si>
+    <t>18:00 WIB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +288,20 @@
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -509,7 +529,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -605,6 +625,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -623,18 +655,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,98 +680,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49139171-CFB2-4DAC-923E-FD0F87B38A94}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6438900" y="3108960"/>
-          <a:ext cx="2164080" cy="441960"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="0" lang="en-US" sz="2400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:uLnTx/>
-              <a:uFillTx/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>18:00 WIB</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -800,65 +733,6 @@
           </a:ext>
         </a:extLst>
       </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2491740</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectangle 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B96E2FF7-36E0-4B16-AC27-AD802D13D9B5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2133600" y="3131820"/>
-          <a:ext cx="2148840" cy="441960"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="2400"/>
-            <a:t>16:30 WIB</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -1250,7 +1124,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5278755" y="2004060"/>
-          <a:ext cx="3364265" cy="811565"/>
+          <a:ext cx="3790985" cy="811565"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1611,7 +1485,7 @@
   <dimension ref="A1:I336"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1619,8 +1493,8 @@
     <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.77734375" style="2" customWidth="1"/>
     <col min="8" max="8" width="13.44140625" style="1" customWidth="1"/>
@@ -2588,26 +2462,26 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="H2" s="24" t="s">
         <v>34</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
       <c r="E4" s="25"/>
@@ -2622,40 +2496,40 @@
       <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="E6" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="35" t="s">
+      <c r="E6" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="34" t="s">
-        <v>38</v>
+      <c r="G6" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="33"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="33"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="36"/>
     </row>
     <row r="10" spans="1:8" ht="13.8" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2717,20 +2591,27 @@
     </row>
     <row r="16" spans="1:8" ht="13.8" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:9" ht="13.8" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="9"/>
+      <c r="E18" s="37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B19" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>18</v>
+      <c r="D19" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="38" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="13.8" x14ac:dyDescent="0.25"/>
@@ -2741,28 +2622,28 @@
     </row>
     <row r="22" spans="2:9" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="E22" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="F22" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="G22" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="H22" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="I22" s="14" t="s">
         <v>24</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="14.4" x14ac:dyDescent="0.25">
@@ -2770,22 +2651,22 @@
         <v>1</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="G23" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="H23" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="14.4" x14ac:dyDescent="0.25">
@@ -2795,7 +2676,7 @@
       <c r="C24" s="15"/>
       <c r="D24" s="16"/>
       <c r="E24" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -2808,7 +2689,7 @@
       <c r="C25" s="15"/>
       <c r="D25" s="16"/>
       <c r="E25" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
@@ -2821,7 +2702,7 @@
       <c r="C26" s="15"/>
       <c r="D26" s="16"/>
       <c r="E26" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
@@ -2834,7 +2715,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="16"/>
       <c r="E27" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -2847,7 +2728,7 @@
       <c r="C28" s="15"/>
       <c r="D28" s="16"/>
       <c r="E28" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
@@ -2860,7 +2741,7 @@
       <c r="C29" s="15"/>
       <c r="D29" s="16"/>
       <c r="E29" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
@@ -2873,7 +2754,7 @@
       <c r="C30" s="15"/>
       <c r="D30" s="16"/>
       <c r="E30" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
@@ -2886,7 +2767,7 @@
       <c r="C31" s="15"/>
       <c r="D31" s="16"/>
       <c r="E31" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
@@ -2899,7 +2780,7 @@
       <c r="C32" s="15"/>
       <c r="D32" s="16"/>
       <c r="E32" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
@@ -2912,7 +2793,7 @@
       <c r="C33" s="15"/>
       <c r="D33" s="16"/>
       <c r="E33" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
@@ -2925,7 +2806,7 @@
       <c r="C34" s="15"/>
       <c r="D34" s="16"/>
       <c r="E34" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
@@ -2938,7 +2819,7 @@
       <c r="C35" s="15"/>
       <c r="D35" s="16"/>
       <c r="E35" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
@@ -2951,7 +2832,7 @@
       <c r="C36" s="15"/>
       <c r="D36" s="16"/>
       <c r="E36" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F36" s="15"/>
       <c r="G36" s="15"/>
@@ -2964,7 +2845,7 @@
       <c r="C37" s="15"/>
       <c r="D37" s="16"/>
       <c r="E37" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
@@ -2977,7 +2858,7 @@
       <c r="C38" s="15"/>
       <c r="D38" s="16"/>
       <c r="E38" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
@@ -2990,7 +2871,7 @@
       <c r="C39" s="15"/>
       <c r="D39" s="16"/>
       <c r="E39" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
@@ -3003,7 +2884,7 @@
       <c r="C40" s="15"/>
       <c r="D40" s="16"/>
       <c r="E40" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F40" s="15"/>
       <c r="G40" s="15"/>
@@ -3016,7 +2897,7 @@
       <c r="C41" s="15"/>
       <c r="D41" s="16"/>
       <c r="E41" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F41" s="15"/>
       <c r="G41" s="15"/>
@@ -3029,7 +2910,7 @@
       <c r="C42" s="15"/>
       <c r="D42" s="16"/>
       <c r="E42" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
@@ -3042,7 +2923,7 @@
       <c r="C43" s="15"/>
       <c r="D43" s="16"/>
       <c r="E43" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F43" s="15"/>
       <c r="G43" s="18"/>
@@ -3055,7 +2936,7 @@
       <c r="C44" s="15"/>
       <c r="D44" s="16"/>
       <c r="E44" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F44" s="15"/>
       <c r="G44" s="18"/>
@@ -3068,7 +2949,7 @@
       <c r="C45" s="15"/>
       <c r="D45" s="16"/>
       <c r="E45" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F45" s="15"/>
       <c r="G45" s="18"/>
@@ -3081,7 +2962,7 @@
       <c r="C46" s="15"/>
       <c r="D46" s="16"/>
       <c r="E46" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F46" s="15"/>
       <c r="G46" s="18"/>
@@ -3094,7 +2975,7 @@
       <c r="C47" s="15"/>
       <c r="D47" s="16"/>
       <c r="E47" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F47" s="15"/>
       <c r="G47" s="18"/>
@@ -3107,7 +2988,7 @@
       <c r="C48" s="15"/>
       <c r="D48" s="16"/>
       <c r="E48" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F48" s="15"/>
       <c r="G48" s="18"/>
@@ -3120,7 +3001,7 @@
       <c r="C49" s="15"/>
       <c r="D49" s="16"/>
       <c r="E49" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F49" s="15"/>
       <c r="G49" s="18"/>
@@ -3133,7 +3014,7 @@
       <c r="C50" s="15"/>
       <c r="D50" s="16"/>
       <c r="E50" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F50" s="15"/>
       <c r="G50" s="18"/>
@@ -3146,7 +3027,7 @@
       <c r="C51" s="15"/>
       <c r="D51" s="16"/>
       <c r="E51" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F51" s="15"/>
       <c r="G51" s="18"/>
@@ -3159,7 +3040,7 @@
       <c r="C52" s="15"/>
       <c r="D52" s="16"/>
       <c r="E52" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F52" s="15"/>
       <c r="G52" s="18"/>
@@ -3172,7 +3053,7 @@
       <c r="C53" s="15"/>
       <c r="D53" s="16"/>
       <c r="E53" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F53" s="15"/>
       <c r="G53" s="18"/>
@@ -3185,7 +3066,7 @@
       <c r="C54" s="15"/>
       <c r="D54" s="16"/>
       <c r="E54" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F54" s="15"/>
       <c r="G54" s="18"/>
@@ -3198,7 +3079,7 @@
       <c r="C55" s="15"/>
       <c r="D55" s="16"/>
       <c r="E55" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F55" s="15"/>
       <c r="G55" s="18"/>
@@ -3211,7 +3092,7 @@
       <c r="C56" s="15"/>
       <c r="D56" s="16"/>
       <c r="E56" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F56" s="15"/>
       <c r="G56" s="18"/>
@@ -3224,7 +3105,7 @@
       <c r="C57" s="15"/>
       <c r="D57" s="16"/>
       <c r="E57" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F57" s="15"/>
       <c r="G57" s="18"/>
@@ -3237,7 +3118,7 @@
       <c r="C58" s="15"/>
       <c r="D58" s="16"/>
       <c r="E58" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F58" s="15"/>
       <c r="G58" s="18"/>
@@ -3250,7 +3131,7 @@
       <c r="C59" s="15"/>
       <c r="D59" s="16"/>
       <c r="E59" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F59" s="15"/>
       <c r="G59" s="18"/>
@@ -3263,7 +3144,7 @@
       <c r="C60" s="15"/>
       <c r="D60" s="16"/>
       <c r="E60" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F60" s="15"/>
       <c r="G60" s="18"/>
@@ -3276,7 +3157,7 @@
       <c r="C61" s="15"/>
       <c r="D61" s="16"/>
       <c r="E61" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F61" s="15"/>
       <c r="G61" s="18"/>
@@ -3289,7 +3170,7 @@
       <c r="C62" s="15"/>
       <c r="D62" s="16"/>
       <c r="E62" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F62" s="15"/>
       <c r="G62" s="18"/>
@@ -3302,7 +3183,7 @@
       <c r="C63" s="15"/>
       <c r="D63" s="16"/>
       <c r="E63" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F63" s="15"/>
       <c r="G63" s="18"/>
@@ -3315,7 +3196,7 @@
       <c r="C64" s="15"/>
       <c r="D64" s="16"/>
       <c r="E64" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F64" s="15"/>
       <c r="G64" s="15"/>
@@ -3328,7 +3209,7 @@
       <c r="C65" s="15"/>
       <c r="D65" s="16"/>
       <c r="E65" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F65" s="15"/>
       <c r="G65" s="15"/>
@@ -3341,7 +3222,7 @@
       <c r="C66" s="15"/>
       <c r="D66" s="16"/>
       <c r="E66" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
@@ -3354,7 +3235,7 @@
       <c r="C67" s="15"/>
       <c r="D67" s="16"/>
       <c r="E67" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F67" s="15"/>
       <c r="G67" s="15"/>
@@ -3367,7 +3248,7 @@
       <c r="C68" s="15"/>
       <c r="D68" s="16"/>
       <c r="E68" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F68" s="15"/>
       <c r="G68" s="15"/>
@@ -3380,7 +3261,7 @@
       <c r="C69" s="15"/>
       <c r="D69" s="16"/>
       <c r="E69" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F69" s="15"/>
       <c r="G69" s="15"/>
@@ -3393,7 +3274,7 @@
       <c r="C70" s="15"/>
       <c r="D70" s="16"/>
       <c r="E70" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F70" s="15"/>
       <c r="G70" s="15"/>
@@ -3406,7 +3287,7 @@
       <c r="C71" s="15"/>
       <c r="D71" s="16"/>
       <c r="E71" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F71" s="15"/>
       <c r="G71" s="15"/>
@@ -3419,7 +3300,7 @@
       <c r="C72" s="15"/>
       <c r="D72" s="16"/>
       <c r="E72" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F72" s="15"/>
       <c r="G72" s="15"/>
@@ -3432,7 +3313,7 @@
       <c r="C73" s="15"/>
       <c r="D73" s="16"/>
       <c r="E73" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F73" s="15"/>
       <c r="G73" s="15"/>
@@ -3445,7 +3326,7 @@
       <c r="C74" s="15"/>
       <c r="D74" s="16"/>
       <c r="E74" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F74" s="15"/>
       <c r="G74" s="15"/>
@@ -3458,7 +3339,7 @@
       <c r="C75" s="15"/>
       <c r="D75" s="16"/>
       <c r="E75" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F75" s="15"/>
       <c r="G75" s="15"/>
@@ -3471,7 +3352,7 @@
       <c r="C76" s="15"/>
       <c r="D76" s="16"/>
       <c r="E76" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F76" s="15"/>
       <c r="G76" s="15"/>
@@ -3484,7 +3365,7 @@
       <c r="C77" s="15"/>
       <c r="D77" s="16"/>
       <c r="E77" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F77" s="15"/>
       <c r="G77" s="15"/>
@@ -3497,7 +3378,7 @@
       <c r="C78" s="15"/>
       <c r="D78" s="16"/>
       <c r="E78" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F78" s="15"/>
       <c r="G78" s="15"/>
@@ -3510,7 +3391,7 @@
       <c r="C79" s="15"/>
       <c r="D79" s="16"/>
       <c r="E79" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F79" s="15"/>
       <c r="G79" s="15"/>
@@ -3523,7 +3404,7 @@
       <c r="C80" s="15"/>
       <c r="D80" s="16"/>
       <c r="E80" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F80" s="15"/>
       <c r="G80" s="15"/>
@@ -3536,7 +3417,7 @@
       <c r="C81" s="15"/>
       <c r="D81" s="16"/>
       <c r="E81" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F81" s="15"/>
       <c r="G81" s="15"/>
@@ -3549,7 +3430,7 @@
       <c r="C82" s="15"/>
       <c r="D82" s="16"/>
       <c r="E82" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F82" s="15"/>
       <c r="G82" s="15"/>
@@ -3562,7 +3443,7 @@
       <c r="C83" s="15"/>
       <c r="D83" s="16"/>
       <c r="E83" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F83" s="15"/>
       <c r="G83" s="15"/>
@@ -3575,7 +3456,7 @@
       <c r="C84" s="15"/>
       <c r="D84" s="16"/>
       <c r="E84" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F84" s="15"/>
       <c r="G84" s="15"/>
@@ -3588,7 +3469,7 @@
       <c r="C85" s="15"/>
       <c r="D85" s="16"/>
       <c r="E85" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F85" s="15"/>
       <c r="G85" s="15"/>
@@ -3601,7 +3482,7 @@
       <c r="C86" s="15"/>
       <c r="D86" s="16"/>
       <c r="E86" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F86" s="15"/>
       <c r="G86" s="15"/>
@@ -3614,7 +3495,7 @@
       <c r="C87" s="15"/>
       <c r="D87" s="16"/>
       <c r="E87" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F87" s="15"/>
       <c r="G87" s="15"/>
@@ -3627,7 +3508,7 @@
       <c r="C88" s="15"/>
       <c r="D88" s="16"/>
       <c r="E88" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F88" s="15"/>
       <c r="G88" s="15"/>
@@ -3640,7 +3521,7 @@
       <c r="C89" s="15"/>
       <c r="D89" s="16"/>
       <c r="E89" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F89" s="15"/>
       <c r="G89" s="15"/>
@@ -3653,7 +3534,7 @@
       <c r="C90" s="15"/>
       <c r="D90" s="16"/>
       <c r="E90" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F90" s="15"/>
       <c r="G90" s="15"/>
@@ -3666,7 +3547,7 @@
       <c r="C91" s="15"/>
       <c r="D91" s="16"/>
       <c r="E91" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F91" s="15"/>
       <c r="G91" s="15"/>
@@ -3679,7 +3560,7 @@
       <c r="C92" s="15"/>
       <c r="D92" s="16"/>
       <c r="E92" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F92" s="15"/>
       <c r="G92" s="15"/>
@@ -3692,7 +3573,7 @@
       <c r="C93" s="15"/>
       <c r="D93" s="16"/>
       <c r="E93" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F93" s="15"/>
       <c r="G93" s="15"/>
@@ -3705,7 +3586,7 @@
       <c r="C94" s="15"/>
       <c r="D94" s="16"/>
       <c r="E94" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F94" s="15"/>
       <c r="G94" s="15"/>
@@ -3718,7 +3599,7 @@
       <c r="C95" s="15"/>
       <c r="D95" s="16"/>
       <c r="E95" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F95" s="15"/>
       <c r="G95" s="15"/>
@@ -3731,7 +3612,7 @@
       <c r="C96" s="15"/>
       <c r="D96" s="16"/>
       <c r="E96" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F96" s="15"/>
       <c r="G96" s="15"/>
@@ -3744,7 +3625,7 @@
       <c r="C97" s="15"/>
       <c r="D97" s="16"/>
       <c r="E97" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F97" s="15"/>
       <c r="G97" s="15"/>
@@ -3757,7 +3638,7 @@
       <c r="C98" s="15"/>
       <c r="D98" s="16"/>
       <c r="E98" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F98" s="15"/>
       <c r="G98" s="15"/>
@@ -3770,7 +3651,7 @@
       <c r="C99" s="15"/>
       <c r="D99" s="16"/>
       <c r="E99" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F99" s="15"/>
       <c r="G99" s="15"/>
@@ -3783,7 +3664,7 @@
       <c r="C100" s="15"/>
       <c r="D100" s="16"/>
       <c r="E100" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F100" s="15"/>
       <c r="G100" s="15"/>
@@ -3796,7 +3677,7 @@
       <c r="C101" s="15"/>
       <c r="D101" s="16"/>
       <c r="E101" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F101" s="15"/>
       <c r="G101" s="15"/>
@@ -3809,7 +3690,7 @@
       <c r="C102" s="15"/>
       <c r="D102" s="16"/>
       <c r="E102" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F102" s="15"/>
       <c r="G102" s="15"/>
@@ -3822,7 +3703,7 @@
       <c r="C103" s="15"/>
       <c r="D103" s="16"/>
       <c r="E103" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F103" s="15"/>
       <c r="G103" s="15"/>
@@ -3835,7 +3716,7 @@
       <c r="C104" s="15"/>
       <c r="D104" s="16"/>
       <c r="E104" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F104" s="15"/>
       <c r="G104" s="15"/>
@@ -3848,7 +3729,7 @@
       <c r="C105" s="15"/>
       <c r="D105" s="16"/>
       <c r="E105" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F105" s="15"/>
       <c r="G105" s="15"/>
@@ -3861,7 +3742,7 @@
       <c r="C106" s="15"/>
       <c r="D106" s="16"/>
       <c r="E106" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F106" s="15"/>
       <c r="G106" s="15"/>
@@ -3874,7 +3755,7 @@
       <c r="C107" s="15"/>
       <c r="D107" s="16"/>
       <c r="E107" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F107" s="15"/>
       <c r="G107" s="15"/>
@@ -3887,7 +3768,7 @@
       <c r="C108" s="15"/>
       <c r="D108" s="16"/>
       <c r="E108" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F108" s="15"/>
       <c r="G108" s="15"/>
@@ -3900,7 +3781,7 @@
       <c r="C109" s="15"/>
       <c r="D109" s="16"/>
       <c r="E109" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F109" s="15"/>
       <c r="G109" s="15"/>
@@ -3913,7 +3794,7 @@
       <c r="C110" s="15"/>
       <c r="D110" s="16"/>
       <c r="E110" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F110" s="15"/>
       <c r="G110" s="15"/>
@@ -3926,7 +3807,7 @@
       <c r="C111" s="15"/>
       <c r="D111" s="16"/>
       <c r="E111" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F111" s="15"/>
       <c r="G111" s="15"/>
@@ -3939,7 +3820,7 @@
       <c r="C112" s="15"/>
       <c r="D112" s="16"/>
       <c r="E112" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F112" s="15"/>
       <c r="G112" s="15"/>
@@ -3952,7 +3833,7 @@
       <c r="C113" s="15"/>
       <c r="D113" s="16"/>
       <c r="E113" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F113" s="15"/>
       <c r="G113" s="15"/>
@@ -3965,7 +3846,7 @@
       <c r="C114" s="15"/>
       <c r="D114" s="16"/>
       <c r="E114" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F114" s="15"/>
       <c r="G114" s="15"/>
@@ -3978,7 +3859,7 @@
       <c r="C115" s="15"/>
       <c r="D115" s="16"/>
       <c r="E115" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F115" s="15"/>
       <c r="G115" s="15"/>
@@ -3991,7 +3872,7 @@
       <c r="C116" s="15"/>
       <c r="D116" s="16"/>
       <c r="E116" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F116" s="15"/>
       <c r="G116" s="15"/>
@@ -4004,7 +3885,7 @@
       <c r="C117" s="15"/>
       <c r="D117" s="16"/>
       <c r="E117" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F117" s="15"/>
       <c r="G117" s="15"/>
@@ -4017,7 +3898,7 @@
       <c r="C118" s="15"/>
       <c r="D118" s="16"/>
       <c r="E118" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F118" s="15"/>
       <c r="G118" s="15"/>
@@ -4030,7 +3911,7 @@
       <c r="C119" s="15"/>
       <c r="D119" s="16"/>
       <c r="E119" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F119" s="15"/>
       <c r="G119" s="15"/>
@@ -4043,7 +3924,7 @@
       <c r="C120" s="15"/>
       <c r="D120" s="16"/>
       <c r="E120" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F120" s="15"/>
       <c r="G120" s="15"/>
@@ -4056,7 +3937,7 @@
       <c r="C121" s="15"/>
       <c r="D121" s="16"/>
       <c r="E121" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F121" s="15"/>
       <c r="G121" s="15"/>
@@ -4069,7 +3950,7 @@
       <c r="C122" s="15"/>
       <c r="D122" s="16"/>
       <c r="E122" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F122" s="15"/>
       <c r="G122" s="15"/>
@@ -4082,7 +3963,7 @@
       <c r="C123" s="15"/>
       <c r="D123" s="16"/>
       <c r="E123" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F123" s="15"/>
       <c r="G123" s="15"/>
@@ -4095,7 +3976,7 @@
       <c r="C124" s="15"/>
       <c r="D124" s="16"/>
       <c r="E124" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F124" s="15"/>
       <c r="G124" s="15"/>
@@ -4108,7 +3989,7 @@
       <c r="C125" s="15"/>
       <c r="D125" s="16"/>
       <c r="E125" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F125" s="15"/>
       <c r="G125" s="15"/>
@@ -4121,7 +4002,7 @@
       <c r="C126" s="15"/>
       <c r="D126" s="16"/>
       <c r="E126" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F126" s="15"/>
       <c r="G126" s="15"/>
@@ -4134,7 +4015,7 @@
       <c r="C127" s="15"/>
       <c r="D127" s="16"/>
       <c r="E127" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F127" s="15"/>
       <c r="G127" s="15"/>
@@ -4147,7 +4028,7 @@
       <c r="C128" s="15"/>
       <c r="D128" s="16"/>
       <c r="E128" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F128" s="15"/>
       <c r="G128" s="15"/>
@@ -4160,7 +4041,7 @@
       <c r="C129" s="15"/>
       <c r="D129" s="16"/>
       <c r="E129" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F129" s="15"/>
       <c r="G129" s="15"/>
@@ -4173,7 +4054,7 @@
       <c r="C130" s="15"/>
       <c r="D130" s="16"/>
       <c r="E130" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F130" s="15"/>
       <c r="G130" s="15"/>
@@ -4186,7 +4067,7 @@
       <c r="C131" s="15"/>
       <c r="D131" s="16"/>
       <c r="E131" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F131" s="15"/>
       <c r="G131" s="15"/>
@@ -4199,7 +4080,7 @@
       <c r="C132" s="15"/>
       <c r="D132" s="16"/>
       <c r="E132" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F132" s="15"/>
       <c r="G132" s="15"/>
@@ -4212,7 +4093,7 @@
       <c r="C133" s="15"/>
       <c r="D133" s="16"/>
       <c r="E133" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F133" s="15"/>
       <c r="G133" s="15"/>
@@ -4225,7 +4106,7 @@
       <c r="C134" s="15"/>
       <c r="D134" s="16"/>
       <c r="E134" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F134" s="15"/>
       <c r="G134" s="15"/>
@@ -4238,7 +4119,7 @@
       <c r="C135" s="15"/>
       <c r="D135" s="16"/>
       <c r="E135" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F135" s="15"/>
       <c r="G135" s="15"/>
@@ -4251,7 +4132,7 @@
       <c r="C136" s="15"/>
       <c r="D136" s="16"/>
       <c r="E136" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F136" s="15"/>
       <c r="G136" s="15"/>
@@ -4264,7 +4145,7 @@
       <c r="C137" s="15"/>
       <c r="D137" s="16"/>
       <c r="E137" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F137" s="15"/>
       <c r="G137" s="15"/>
@@ -4277,7 +4158,7 @@
       <c r="C138" s="15"/>
       <c r="D138" s="16"/>
       <c r="E138" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F138" s="15"/>
       <c r="G138" s="15"/>
@@ -4290,7 +4171,7 @@
       <c r="C139" s="15"/>
       <c r="D139" s="16"/>
       <c r="E139" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F139" s="15"/>
       <c r="G139" s="15"/>
@@ -4303,7 +4184,7 @@
       <c r="C140" s="15"/>
       <c r="D140" s="16"/>
       <c r="E140" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F140" s="15"/>
       <c r="G140" s="15"/>
@@ -4316,7 +4197,7 @@
       <c r="C141" s="15"/>
       <c r="D141" s="16"/>
       <c r="E141" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F141" s="15"/>
       <c r="G141" s="15"/>
@@ -4329,7 +4210,7 @@
       <c r="C142" s="15"/>
       <c r="D142" s="16"/>
       <c r="E142" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F142" s="15"/>
       <c r="G142" s="15"/>
@@ -4342,7 +4223,7 @@
       <c r="C143" s="15"/>
       <c r="D143" s="16"/>
       <c r="E143" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F143" s="15"/>
       <c r="G143" s="15"/>
@@ -4355,7 +4236,7 @@
       <c r="C144" s="15"/>
       <c r="D144" s="16"/>
       <c r="E144" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F144" s="15"/>
       <c r="G144" s="15"/>
@@ -4368,7 +4249,7 @@
       <c r="C145" s="15"/>
       <c r="D145" s="16"/>
       <c r="E145" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F145" s="15"/>
       <c r="G145" s="15"/>
@@ -4381,7 +4262,7 @@
       <c r="C146" s="15"/>
       <c r="D146" s="16"/>
       <c r="E146" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F146" s="15"/>
       <c r="G146" s="15"/>
@@ -4394,7 +4275,7 @@
       <c r="C147" s="15"/>
       <c r="D147" s="16"/>
       <c r="E147" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F147" s="15"/>
       <c r="G147" s="15"/>
@@ -4407,7 +4288,7 @@
       <c r="C148" s="15"/>
       <c r="D148" s="16"/>
       <c r="E148" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F148" s="15"/>
       <c r="G148" s="15"/>
@@ -4420,7 +4301,7 @@
       <c r="C149" s="15"/>
       <c r="D149" s="16"/>
       <c r="E149" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F149" s="15"/>
       <c r="G149" s="15"/>
@@ -4433,7 +4314,7 @@
       <c r="C150" s="15"/>
       <c r="D150" s="16"/>
       <c r="E150" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F150" s="15"/>
       <c r="G150" s="15"/>
@@ -4446,7 +4327,7 @@
       <c r="C151" s="15"/>
       <c r="D151" s="16"/>
       <c r="E151" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F151" s="15"/>
       <c r="G151" s="15"/>
@@ -4459,7 +4340,7 @@
       <c r="C152" s="15"/>
       <c r="D152" s="16"/>
       <c r="E152" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F152" s="15"/>
       <c r="G152" s="15"/>
@@ -4472,7 +4353,7 @@
       <c r="C153" s="15"/>
       <c r="D153" s="16"/>
       <c r="E153" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F153" s="15"/>
       <c r="G153" s="15"/>
@@ -4485,7 +4366,7 @@
       <c r="C154" s="15"/>
       <c r="D154" s="16"/>
       <c r="E154" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F154" s="15"/>
       <c r="G154" s="15"/>
@@ -4498,7 +4379,7 @@
       <c r="C155" s="15"/>
       <c r="D155" s="16"/>
       <c r="E155" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F155" s="15"/>
       <c r="G155" s="15"/>
@@ -4511,7 +4392,7 @@
       <c r="C156" s="15"/>
       <c r="D156" s="16"/>
       <c r="E156" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F156" s="15"/>
       <c r="G156" s="15"/>
@@ -4524,7 +4405,7 @@
       <c r="C157" s="15"/>
       <c r="D157" s="16"/>
       <c r="E157" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F157" s="15"/>
       <c r="G157" s="15"/>
@@ -4537,7 +4418,7 @@
       <c r="C158" s="15"/>
       <c r="D158" s="16"/>
       <c r="E158" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F158" s="15"/>
       <c r="G158" s="15"/>
@@ -4550,7 +4431,7 @@
       <c r="C159" s="15"/>
       <c r="D159" s="16"/>
       <c r="E159" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F159" s="15"/>
       <c r="G159" s="15"/>
@@ -4563,7 +4444,7 @@
       <c r="C160" s="15"/>
       <c r="D160" s="16"/>
       <c r="E160" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F160" s="15"/>
       <c r="G160" s="15"/>
@@ -4576,7 +4457,7 @@
       <c r="C161" s="15"/>
       <c r="D161" s="16"/>
       <c r="E161" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F161" s="15"/>
       <c r="G161" s="15"/>
@@ -4589,7 +4470,7 @@
       <c r="C162" s="15"/>
       <c r="D162" s="16"/>
       <c r="E162" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F162" s="15"/>
       <c r="G162" s="15"/>
@@ -4602,7 +4483,7 @@
       <c r="C163" s="15"/>
       <c r="D163" s="16"/>
       <c r="E163" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F163" s="15"/>
       <c r="G163" s="15"/>
@@ -4615,7 +4496,7 @@
       <c r="C164" s="15"/>
       <c r="D164" s="16"/>
       <c r="E164" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F164" s="15"/>
       <c r="G164" s="15"/>
@@ -4628,7 +4509,7 @@
       <c r="C165" s="15"/>
       <c r="D165" s="16"/>
       <c r="E165" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F165" s="15"/>
       <c r="G165" s="15"/>
@@ -4641,7 +4522,7 @@
       <c r="C166" s="15"/>
       <c r="D166" s="16"/>
       <c r="E166" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F166" s="15"/>
       <c r="G166" s="15"/>
@@ -4654,7 +4535,7 @@
       <c r="C167" s="15"/>
       <c r="D167" s="16"/>
       <c r="E167" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F167" s="15"/>
       <c r="G167" s="15"/>
@@ -4667,7 +4548,7 @@
       <c r="C168" s="15"/>
       <c r="D168" s="16"/>
       <c r="E168" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F168" s="15"/>
       <c r="G168" s="15"/>
@@ -4680,7 +4561,7 @@
       <c r="C169" s="15"/>
       <c r="D169" s="16"/>
       <c r="E169" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F169" s="15"/>
       <c r="G169" s="15"/>
@@ -4693,7 +4574,7 @@
       <c r="C170" s="15"/>
       <c r="D170" s="16"/>
       <c r="E170" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F170" s="15"/>
       <c r="G170" s="15"/>
@@ -4706,7 +4587,7 @@
       <c r="C171" s="15"/>
       <c r="D171" s="16"/>
       <c r="E171" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F171" s="15"/>
       <c r="G171" s="15"/>
@@ -4719,7 +4600,7 @@
       <c r="C172" s="15"/>
       <c r="D172" s="16"/>
       <c r="E172" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F172" s="15"/>
       <c r="G172" s="15"/>
@@ -4732,7 +4613,7 @@
       <c r="C173" s="15"/>
       <c r="D173" s="16"/>
       <c r="E173" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F173" s="15"/>
       <c r="G173" s="15"/>
@@ -4745,7 +4626,7 @@
       <c r="C174" s="15"/>
       <c r="D174" s="16"/>
       <c r="E174" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F174" s="15"/>
       <c r="G174" s="15"/>
@@ -4758,7 +4639,7 @@
       <c r="C175" s="15"/>
       <c r="D175" s="16"/>
       <c r="E175" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F175" s="15"/>
       <c r="G175" s="15"/>
@@ -4771,7 +4652,7 @@
       <c r="C176" s="15"/>
       <c r="D176" s="16"/>
       <c r="E176" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F176" s="15"/>
       <c r="G176" s="15"/>
@@ -4784,7 +4665,7 @@
       <c r="C177" s="15"/>
       <c r="D177" s="16"/>
       <c r="E177" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F177" s="15"/>
       <c r="G177" s="15"/>
@@ -4797,7 +4678,7 @@
       <c r="C178" s="15"/>
       <c r="D178" s="16"/>
       <c r="E178" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F178" s="15"/>
       <c r="G178" s="15"/>
@@ -4810,7 +4691,7 @@
       <c r="C179" s="15"/>
       <c r="D179" s="16"/>
       <c r="E179" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F179" s="15"/>
       <c r="G179" s="15"/>
@@ -4823,7 +4704,7 @@
       <c r="C180" s="15"/>
       <c r="D180" s="16"/>
       <c r="E180" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F180" s="15"/>
       <c r="G180" s="15"/>
@@ -4836,7 +4717,7 @@
       <c r="C181" s="15"/>
       <c r="D181" s="16"/>
       <c r="E181" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F181" s="15"/>
       <c r="G181" s="15"/>
@@ -4849,7 +4730,7 @@
       <c r="C182" s="15"/>
       <c r="D182" s="16"/>
       <c r="E182" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F182" s="15"/>
       <c r="G182" s="15"/>
@@ -4862,7 +4743,7 @@
       <c r="C183" s="15"/>
       <c r="D183" s="16"/>
       <c r="E183" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F183" s="15"/>
       <c r="G183" s="15"/>
@@ -4875,7 +4756,7 @@
       <c r="C184" s="15"/>
       <c r="D184" s="16"/>
       <c r="E184" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F184" s="15"/>
       <c r="G184" s="15"/>
@@ -4888,7 +4769,7 @@
       <c r="C185" s="15"/>
       <c r="D185" s="16"/>
       <c r="E185" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F185" s="15"/>
       <c r="G185" s="15"/>
@@ -4901,7 +4782,7 @@
       <c r="C186" s="15"/>
       <c r="D186" s="16"/>
       <c r="E186" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F186" s="15"/>
       <c r="G186" s="15"/>
@@ -4914,7 +4795,7 @@
       <c r="C187" s="15"/>
       <c r="D187" s="16"/>
       <c r="E187" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F187" s="15"/>
       <c r="G187" s="15"/>
@@ -4927,7 +4808,7 @@
       <c r="C188" s="15"/>
       <c r="D188" s="16"/>
       <c r="E188" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F188" s="15"/>
       <c r="G188" s="15"/>
@@ -4940,7 +4821,7 @@
       <c r="C189" s="15"/>
       <c r="D189" s="16"/>
       <c r="E189" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F189" s="15"/>
       <c r="G189" s="15"/>
@@ -4953,7 +4834,7 @@
       <c r="C190" s="15"/>
       <c r="D190" s="16"/>
       <c r="E190" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F190" s="15"/>
       <c r="G190" s="15"/>
@@ -4966,7 +4847,7 @@
       <c r="C191" s="15"/>
       <c r="D191" s="16"/>
       <c r="E191" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F191" s="15"/>
       <c r="G191" s="15"/>
@@ -4979,7 +4860,7 @@
       <c r="C192" s="15"/>
       <c r="D192" s="16"/>
       <c r="E192" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F192" s="15"/>
       <c r="G192" s="15"/>
@@ -4992,7 +4873,7 @@
       <c r="C193" s="15"/>
       <c r="D193" s="16"/>
       <c r="E193" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F193" s="15"/>
       <c r="G193" s="15"/>
@@ -5005,7 +4886,7 @@
       <c r="C194" s="15"/>
       <c r="D194" s="16"/>
       <c r="E194" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F194" s="15"/>
       <c r="G194" s="15"/>
@@ -5018,7 +4899,7 @@
       <c r="C195" s="15"/>
       <c r="D195" s="16"/>
       <c r="E195" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F195" s="15"/>
       <c r="G195" s="15"/>
@@ -5031,7 +4912,7 @@
       <c r="C196" s="15"/>
       <c r="D196" s="16"/>
       <c r="E196" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F196" s="15"/>
       <c r="G196" s="15"/>
@@ -5044,7 +4925,7 @@
       <c r="C197" s="15"/>
       <c r="D197" s="16"/>
       <c r="E197" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F197" s="15"/>
       <c r="G197" s="15"/>
@@ -5057,7 +4938,7 @@
       <c r="C198" s="15"/>
       <c r="D198" s="16"/>
       <c r="E198" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F198" s="15"/>
       <c r="G198" s="15"/>
@@ -5070,7 +4951,7 @@
       <c r="C199" s="15"/>
       <c r="D199" s="16"/>
       <c r="E199" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F199" s="15"/>
       <c r="G199" s="15"/>
@@ -5083,7 +4964,7 @@
       <c r="C200" s="15"/>
       <c r="D200" s="16"/>
       <c r="E200" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F200" s="15"/>
       <c r="G200" s="15"/>
@@ -5096,7 +4977,7 @@
       <c r="C201" s="15"/>
       <c r="D201" s="16"/>
       <c r="E201" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F201" s="15"/>
       <c r="G201" s="15"/>
@@ -5109,7 +4990,7 @@
       <c r="C202" s="15"/>
       <c r="D202" s="16"/>
       <c r="E202" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F202" s="15"/>
       <c r="G202" s="15"/>
@@ -5122,7 +5003,7 @@
       <c r="C203" s="15"/>
       <c r="D203" s="16"/>
       <c r="E203" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F203" s="15"/>
       <c r="G203" s="15"/>
@@ -5135,7 +5016,7 @@
       <c r="C204" s="15"/>
       <c r="D204" s="16"/>
       <c r="E204" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F204" s="15"/>
       <c r="G204" s="15"/>
@@ -5148,7 +5029,7 @@
       <c r="C205" s="15"/>
       <c r="D205" s="16"/>
       <c r="E205" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F205" s="15"/>
       <c r="G205" s="15"/>
@@ -5161,7 +5042,7 @@
       <c r="C206" s="15"/>
       <c r="D206" s="16"/>
       <c r="E206" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F206" s="15"/>
       <c r="G206" s="15"/>
@@ -5174,7 +5055,7 @@
       <c r="C207" s="15"/>
       <c r="D207" s="16"/>
       <c r="E207" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F207" s="15"/>
       <c r="G207" s="15"/>
@@ -5187,7 +5068,7 @@
       <c r="C208" s="15"/>
       <c r="D208" s="16"/>
       <c r="E208" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F208" s="15"/>
       <c r="G208" s="15"/>
@@ -5200,7 +5081,7 @@
       <c r="C209" s="15"/>
       <c r="D209" s="16"/>
       <c r="E209" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F209" s="15"/>
       <c r="G209" s="15"/>
@@ -5213,7 +5094,7 @@
       <c r="C210" s="15"/>
       <c r="D210" s="16"/>
       <c r="E210" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F210" s="15"/>
       <c r="G210" s="15"/>
@@ -5226,7 +5107,7 @@
       <c r="C211" s="15"/>
       <c r="D211" s="16"/>
       <c r="E211" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F211" s="15"/>
       <c r="G211" s="15"/>
@@ -5239,7 +5120,7 @@
       <c r="C212" s="15"/>
       <c r="D212" s="16"/>
       <c r="E212" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F212" s="15"/>
       <c r="G212" s="15"/>
@@ -5252,7 +5133,7 @@
       <c r="C213" s="15"/>
       <c r="D213" s="16"/>
       <c r="E213" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F213" s="15"/>
       <c r="G213" s="15"/>
@@ -5265,7 +5146,7 @@
       <c r="C214" s="15"/>
       <c r="D214" s="16"/>
       <c r="E214" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F214" s="15"/>
       <c r="G214" s="15"/>
@@ -5278,7 +5159,7 @@
       <c r="C215" s="15"/>
       <c r="D215" s="16"/>
       <c r="E215" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F215" s="15"/>
       <c r="G215" s="15"/>
@@ -5291,7 +5172,7 @@
       <c r="C216" s="15"/>
       <c r="D216" s="16"/>
       <c r="E216" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F216" s="15"/>
       <c r="G216" s="15"/>
@@ -5304,7 +5185,7 @@
       <c r="C217" s="15"/>
       <c r="D217" s="16"/>
       <c r="E217" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F217" s="15"/>
       <c r="G217" s="15"/>
@@ -5317,7 +5198,7 @@
       <c r="C218" s="15"/>
       <c r="D218" s="16"/>
       <c r="E218" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F218" s="15"/>
       <c r="G218" s="15"/>
@@ -5330,7 +5211,7 @@
       <c r="C219" s="15"/>
       <c r="D219" s="16"/>
       <c r="E219" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F219" s="15"/>
       <c r="G219" s="15"/>
@@ -5343,7 +5224,7 @@
       <c r="C220" s="15"/>
       <c r="D220" s="16"/>
       <c r="E220" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F220" s="15"/>
       <c r="G220" s="15"/>
@@ -5356,7 +5237,7 @@
       <c r="C221" s="15"/>
       <c r="D221" s="16"/>
       <c r="E221" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F221" s="15"/>
       <c r="G221" s="15"/>
@@ -5369,7 +5250,7 @@
       <c r="C222" s="15"/>
       <c r="D222" s="16"/>
       <c r="E222" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F222" s="15"/>
       <c r="G222" s="15"/>
@@ -5382,7 +5263,7 @@
       <c r="C223" s="15"/>
       <c r="D223" s="16"/>
       <c r="E223" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F223" s="15"/>
       <c r="G223" s="15"/>
@@ -5395,7 +5276,7 @@
       <c r="C224" s="15"/>
       <c r="D224" s="16"/>
       <c r="E224" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F224" s="15"/>
       <c r="G224" s="15"/>
@@ -5408,7 +5289,7 @@
       <c r="C225" s="15"/>
       <c r="D225" s="16"/>
       <c r="E225" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F225" s="15"/>
       <c r="G225" s="15"/>
@@ -5421,7 +5302,7 @@
       <c r="C226" s="15"/>
       <c r="D226" s="16"/>
       <c r="E226" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F226" s="15"/>
       <c r="G226" s="15"/>
@@ -5434,7 +5315,7 @@
       <c r="C227" s="15"/>
       <c r="D227" s="16"/>
       <c r="E227" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F227" s="15"/>
       <c r="G227" s="15"/>
@@ -5447,7 +5328,7 @@
       <c r="C228" s="15"/>
       <c r="D228" s="16"/>
       <c r="E228" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F228" s="15"/>
       <c r="G228" s="15"/>
@@ -5460,7 +5341,7 @@
       <c r="C229" s="15"/>
       <c r="D229" s="16"/>
       <c r="E229" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F229" s="15"/>
       <c r="G229" s="15"/>
@@ -5473,7 +5354,7 @@
       <c r="C230" s="15"/>
       <c r="D230" s="16"/>
       <c r="E230" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F230" s="15"/>
       <c r="G230" s="15"/>
@@ -5486,7 +5367,7 @@
       <c r="C231" s="15"/>
       <c r="D231" s="16"/>
       <c r="E231" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F231" s="15"/>
       <c r="G231" s="15"/>
@@ -5499,7 +5380,7 @@
       <c r="C232" s="15"/>
       <c r="D232" s="16"/>
       <c r="E232" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F232" s="15"/>
       <c r="G232" s="15"/>
@@ -5512,7 +5393,7 @@
       <c r="C233" s="15"/>
       <c r="D233" s="16"/>
       <c r="E233" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F233" s="15"/>
       <c r="G233" s="15"/>
@@ -5525,7 +5406,7 @@
       <c r="C234" s="15"/>
       <c r="D234" s="16"/>
       <c r="E234" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F234" s="15"/>
       <c r="G234" s="15"/>
@@ -5538,7 +5419,7 @@
       <c r="C235" s="15"/>
       <c r="D235" s="16"/>
       <c r="E235" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F235" s="15"/>
       <c r="G235" s="15"/>
@@ -5551,7 +5432,7 @@
       <c r="C236" s="15"/>
       <c r="D236" s="16"/>
       <c r="E236" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F236" s="15"/>
       <c r="G236" s="15"/>
@@ -5564,7 +5445,7 @@
       <c r="C237" s="15"/>
       <c r="D237" s="16"/>
       <c r="E237" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F237" s="15"/>
       <c r="G237" s="15"/>
@@ -5577,7 +5458,7 @@
       <c r="C238" s="15"/>
       <c r="D238" s="16"/>
       <c r="E238" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F238" s="15"/>
       <c r="G238" s="15"/>
@@ -5590,7 +5471,7 @@
       <c r="C239" s="15"/>
       <c r="D239" s="16"/>
       <c r="E239" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F239" s="15"/>
       <c r="G239" s="15"/>
@@ -5603,7 +5484,7 @@
       <c r="C240" s="15"/>
       <c r="D240" s="16"/>
       <c r="E240" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F240" s="15"/>
       <c r="G240" s="15"/>
@@ -5616,7 +5497,7 @@
       <c r="C241" s="15"/>
       <c r="D241" s="16"/>
       <c r="E241" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F241" s="15"/>
       <c r="G241" s="15"/>
@@ -5629,7 +5510,7 @@
       <c r="C242" s="15"/>
       <c r="D242" s="16"/>
       <c r="E242" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F242" s="15"/>
       <c r="G242" s="15"/>
@@ -5642,7 +5523,7 @@
       <c r="C243" s="15"/>
       <c r="D243" s="16"/>
       <c r="E243" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F243" s="15"/>
       <c r="G243" s="15"/>
@@ -5655,7 +5536,7 @@
       <c r="C244" s="15"/>
       <c r="D244" s="16"/>
       <c r="E244" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F244" s="15"/>
       <c r="G244" s="15"/>
@@ -5668,7 +5549,7 @@
       <c r="C245" s="15"/>
       <c r="D245" s="16"/>
       <c r="E245" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F245" s="15"/>
       <c r="G245" s="15"/>
@@ -5681,7 +5562,7 @@
       <c r="C246" s="15"/>
       <c r="D246" s="16"/>
       <c r="E246" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F246" s="15"/>
       <c r="G246" s="15"/>
@@ -5694,7 +5575,7 @@
       <c r="C247" s="15"/>
       <c r="D247" s="16"/>
       <c r="E247" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F247" s="15"/>
       <c r="G247" s="15"/>
@@ -5707,7 +5588,7 @@
       <c r="C248" s="15"/>
       <c r="D248" s="16"/>
       <c r="E248" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F248" s="15"/>
       <c r="G248" s="15"/>
@@ -5720,7 +5601,7 @@
       <c r="C249" s="15"/>
       <c r="D249" s="16"/>
       <c r="E249" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F249" s="15"/>
       <c r="G249" s="15"/>
@@ -5733,7 +5614,7 @@
       <c r="C250" s="15"/>
       <c r="D250" s="16"/>
       <c r="E250" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F250" s="15"/>
       <c r="G250" s="15"/>
@@ -5746,7 +5627,7 @@
       <c r="C251" s="15"/>
       <c r="D251" s="16"/>
       <c r="E251" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F251" s="15"/>
       <c r="G251" s="15"/>
@@ -5759,7 +5640,7 @@
       <c r="C252" s="15"/>
       <c r="D252" s="16"/>
       <c r="E252" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F252" s="15"/>
       <c r="G252" s="15"/>
@@ -5772,7 +5653,7 @@
       <c r="C253" s="15"/>
       <c r="D253" s="16"/>
       <c r="E253" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F253" s="15"/>
       <c r="G253" s="15"/>
@@ -5785,7 +5666,7 @@
       <c r="C254" s="15"/>
       <c r="D254" s="16"/>
       <c r="E254" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F254" s="15"/>
       <c r="G254" s="15"/>
@@ -5798,7 +5679,7 @@
       <c r="C255" s="15"/>
       <c r="D255" s="16"/>
       <c r="E255" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F255" s="15"/>
       <c r="G255" s="15"/>
@@ -5811,7 +5692,7 @@
       <c r="C256" s="15"/>
       <c r="D256" s="16"/>
       <c r="E256" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F256" s="15"/>
       <c r="G256" s="15"/>
@@ -5824,7 +5705,7 @@
       <c r="C257" s="15"/>
       <c r="D257" s="16"/>
       <c r="E257" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F257" s="15"/>
       <c r="G257" s="15"/>
@@ -5837,7 +5718,7 @@
       <c r="C258" s="15"/>
       <c r="D258" s="16"/>
       <c r="E258" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F258" s="15"/>
       <c r="G258" s="15"/>
@@ -5850,7 +5731,7 @@
       <c r="C259" s="15"/>
       <c r="D259" s="16"/>
       <c r="E259" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F259" s="15"/>
       <c r="G259" s="15"/>
@@ -5863,7 +5744,7 @@
       <c r="C260" s="15"/>
       <c r="D260" s="16"/>
       <c r="E260" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F260" s="15"/>
       <c r="G260" s="15"/>
@@ -5876,7 +5757,7 @@
       <c r="C261" s="15"/>
       <c r="D261" s="16"/>
       <c r="E261" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F261" s="15"/>
       <c r="G261" s="15"/>
@@ -5889,7 +5770,7 @@
       <c r="C262" s="15"/>
       <c r="D262" s="16"/>
       <c r="E262" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F262" s="15"/>
       <c r="G262" s="15"/>
@@ -5902,7 +5783,7 @@
       <c r="C263" s="15"/>
       <c r="D263" s="16"/>
       <c r="E263" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F263" s="15"/>
       <c r="G263" s="15"/>
@@ -5915,7 +5796,7 @@
       <c r="C264" s="15"/>
       <c r="D264" s="16"/>
       <c r="E264" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F264" s="15"/>
       <c r="G264" s="15"/>
@@ -5928,7 +5809,7 @@
       <c r="C265" s="15"/>
       <c r="D265" s="16"/>
       <c r="E265" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F265" s="15"/>
       <c r="G265" s="15"/>
@@ -5941,7 +5822,7 @@
       <c r="C266" s="15"/>
       <c r="D266" s="16"/>
       <c r="E266" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F266" s="15"/>
       <c r="G266" s="15"/>
@@ -5954,7 +5835,7 @@
       <c r="C267" s="15"/>
       <c r="D267" s="16"/>
       <c r="E267" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F267" s="15"/>
       <c r="G267" s="15"/>
@@ -5967,7 +5848,7 @@
       <c r="C268" s="15"/>
       <c r="D268" s="16"/>
       <c r="E268" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F268" s="15"/>
       <c r="G268" s="15"/>
@@ -5980,7 +5861,7 @@
       <c r="C269" s="15"/>
       <c r="D269" s="16"/>
       <c r="E269" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F269" s="15"/>
       <c r="G269" s="15"/>
@@ -5993,7 +5874,7 @@
       <c r="C270" s="15"/>
       <c r="D270" s="16"/>
       <c r="E270" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F270" s="15"/>
       <c r="G270" s="15"/>
@@ -6006,7 +5887,7 @@
       <c r="C271" s="15"/>
       <c r="D271" s="16"/>
       <c r="E271" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F271" s="15"/>
       <c r="G271" s="15"/>
@@ -6019,7 +5900,7 @@
       <c r="C272" s="15"/>
       <c r="D272" s="16"/>
       <c r="E272" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F272" s="15"/>
       <c r="G272" s="15"/>
@@ -6032,7 +5913,7 @@
       <c r="C273" s="15"/>
       <c r="D273" s="16"/>
       <c r="E273" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F273" s="15"/>
       <c r="G273" s="15"/>
@@ -6045,7 +5926,7 @@
       <c r="C274" s="15"/>
       <c r="D274" s="16"/>
       <c r="E274" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F274" s="15"/>
       <c r="G274" s="15"/>
@@ -6058,7 +5939,7 @@
       <c r="C275" s="15"/>
       <c r="D275" s="16"/>
       <c r="E275" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F275" s="15"/>
       <c r="G275" s="15"/>
@@ -6071,7 +5952,7 @@
       <c r="C276" s="15"/>
       <c r="D276" s="16"/>
       <c r="E276" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F276" s="15"/>
       <c r="G276" s="15"/>
@@ -6084,7 +5965,7 @@
       <c r="C277" s="15"/>
       <c r="D277" s="16"/>
       <c r="E277" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F277" s="15"/>
       <c r="G277" s="15"/>
@@ -6097,7 +5978,7 @@
       <c r="C278" s="15"/>
       <c r="D278" s="16"/>
       <c r="E278" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F278" s="15"/>
       <c r="G278" s="15"/>
@@ -6110,7 +5991,7 @@
       <c r="C279" s="15"/>
       <c r="D279" s="16"/>
       <c r="E279" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F279" s="15"/>
       <c r="G279" s="15"/>
@@ -6123,7 +6004,7 @@
       <c r="C280" s="15"/>
       <c r="D280" s="16"/>
       <c r="E280" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F280" s="15"/>
       <c r="G280" s="15"/>
@@ -6136,7 +6017,7 @@
       <c r="C281" s="15"/>
       <c r="D281" s="16"/>
       <c r="E281" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F281" s="15"/>
       <c r="G281" s="15"/>
@@ -6149,7 +6030,7 @@
       <c r="C282" s="15"/>
       <c r="D282" s="16"/>
       <c r="E282" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F282" s="15"/>
       <c r="G282" s="15"/>
@@ -6162,7 +6043,7 @@
       <c r="C283" s="15"/>
       <c r="D283" s="16"/>
       <c r="E283" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F283" s="15"/>
       <c r="G283" s="15"/>
@@ -6175,7 +6056,7 @@
       <c r="C284" s="15"/>
       <c r="D284" s="16"/>
       <c r="E284" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F284" s="15"/>
       <c r="G284" s="15"/>
@@ -6188,7 +6069,7 @@
       <c r="C285" s="15"/>
       <c r="D285" s="16"/>
       <c r="E285" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F285" s="15"/>
       <c r="G285" s="15"/>
@@ -6201,7 +6082,7 @@
       <c r="C286" s="15"/>
       <c r="D286" s="16"/>
       <c r="E286" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F286" s="15"/>
       <c r="G286" s="15"/>
@@ -6214,7 +6095,7 @@
       <c r="C287" s="15"/>
       <c r="D287" s="16"/>
       <c r="E287" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F287" s="15"/>
       <c r="G287" s="15"/>
@@ -6227,7 +6108,7 @@
       <c r="C288" s="15"/>
       <c r="D288" s="16"/>
       <c r="E288" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F288" s="15"/>
       <c r="G288" s="15"/>
@@ -6240,7 +6121,7 @@
       <c r="C289" s="15"/>
       <c r="D289" s="16"/>
       <c r="E289" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F289" s="15"/>
       <c r="G289" s="15"/>
@@ -6253,7 +6134,7 @@
       <c r="C290" s="15"/>
       <c r="D290" s="16"/>
       <c r="E290" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F290" s="15"/>
       <c r="G290" s="15"/>
@@ -6266,7 +6147,7 @@
       <c r="C291" s="15"/>
       <c r="D291" s="16"/>
       <c r="E291" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F291" s="15"/>
       <c r="G291" s="15"/>
@@ -6279,7 +6160,7 @@
       <c r="C292" s="15"/>
       <c r="D292" s="16"/>
       <c r="E292" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F292" s="15"/>
       <c r="G292" s="15"/>
@@ -6292,7 +6173,7 @@
       <c r="C293" s="15"/>
       <c r="D293" s="16"/>
       <c r="E293" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F293" s="15"/>
       <c r="G293" s="15"/>
@@ -6305,7 +6186,7 @@
       <c r="C294" s="15"/>
       <c r="D294" s="16"/>
       <c r="E294" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F294" s="15"/>
       <c r="G294" s="15"/>
@@ -6318,7 +6199,7 @@
       <c r="C295" s="15"/>
       <c r="D295" s="16"/>
       <c r="E295" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F295" s="15"/>
       <c r="G295" s="15"/>
@@ -6331,7 +6212,7 @@
       <c r="C296" s="15"/>
       <c r="D296" s="16"/>
       <c r="E296" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F296" s="15"/>
       <c r="G296" s="15"/>
@@ -6344,7 +6225,7 @@
       <c r="C297" s="15"/>
       <c r="D297" s="16"/>
       <c r="E297" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F297" s="15"/>
       <c r="G297" s="15"/>
@@ -6357,7 +6238,7 @@
       <c r="C298" s="15"/>
       <c r="D298" s="16"/>
       <c r="E298" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F298" s="15"/>
       <c r="G298" s="15"/>
@@ -6370,7 +6251,7 @@
       <c r="C299" s="15"/>
       <c r="D299" s="16"/>
       <c r="E299" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F299" s="15"/>
       <c r="G299" s="15"/>
@@ -6383,7 +6264,7 @@
       <c r="C300" s="15"/>
       <c r="D300" s="16"/>
       <c r="E300" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F300" s="15"/>
       <c r="G300" s="15"/>
@@ -6396,7 +6277,7 @@
       <c r="C301" s="15"/>
       <c r="D301" s="16"/>
       <c r="E301" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F301" s="15"/>
       <c r="G301" s="15"/>
@@ -6409,7 +6290,7 @@
       <c r="C302" s="15"/>
       <c r="D302" s="16"/>
       <c r="E302" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F302" s="15"/>
       <c r="G302" s="15"/>
@@ -6422,7 +6303,7 @@
       <c r="C303" s="15"/>
       <c r="D303" s="16"/>
       <c r="E303" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F303" s="15"/>
       <c r="G303" s="15"/>
@@ -6435,7 +6316,7 @@
       <c r="C304" s="15"/>
       <c r="D304" s="16"/>
       <c r="E304" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F304" s="15"/>
       <c r="G304" s="15"/>
@@ -6448,7 +6329,7 @@
       <c r="C305" s="15"/>
       <c r="D305" s="16"/>
       <c r="E305" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F305" s="15"/>
       <c r="G305" s="15"/>
@@ -6461,7 +6342,7 @@
       <c r="C306" s="15"/>
       <c r="D306" s="16"/>
       <c r="E306" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F306" s="15"/>
       <c r="G306" s="15"/>
@@ -6474,7 +6355,7 @@
       <c r="C307" s="15"/>
       <c r="D307" s="16"/>
       <c r="E307" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F307" s="15"/>
       <c r="G307" s="15"/>
@@ -6487,7 +6368,7 @@
       <c r="C308" s="15"/>
       <c r="D308" s="16"/>
       <c r="E308" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F308" s="15"/>
       <c r="G308" s="15"/>
@@ -6500,7 +6381,7 @@
       <c r="C309" s="15"/>
       <c r="D309" s="16"/>
       <c r="E309" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F309" s="15"/>
       <c r="G309" s="15"/>
@@ -6513,7 +6394,7 @@
       <c r="C310" s="15"/>
       <c r="D310" s="16"/>
       <c r="E310" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F310" s="15"/>
       <c r="G310" s="15"/>
@@ -6526,7 +6407,7 @@
       <c r="C311" s="15"/>
       <c r="D311" s="16"/>
       <c r="E311" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F311" s="15"/>
       <c r="G311" s="15"/>
@@ -6539,7 +6420,7 @@
       <c r="C312" s="15"/>
       <c r="D312" s="16"/>
       <c r="E312" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F312" s="15"/>
       <c r="G312" s="15"/>
@@ -6552,7 +6433,7 @@
       <c r="C313" s="15"/>
       <c r="D313" s="16"/>
       <c r="E313" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F313" s="15"/>
       <c r="G313" s="15"/>
@@ -6565,7 +6446,7 @@
       <c r="C314" s="15"/>
       <c r="D314" s="16"/>
       <c r="E314" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F314" s="15"/>
       <c r="G314" s="15"/>
@@ -6578,7 +6459,7 @@
       <c r="C315" s="15"/>
       <c r="D315" s="16"/>
       <c r="E315" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F315" s="15"/>
       <c r="G315" s="15"/>
@@ -6591,7 +6472,7 @@
       <c r="C316" s="15"/>
       <c r="D316" s="16"/>
       <c r="E316" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F316" s="15"/>
       <c r="G316" s="15"/>
@@ -6604,7 +6485,7 @@
       <c r="C317" s="15"/>
       <c r="D317" s="16"/>
       <c r="E317" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F317" s="15"/>
       <c r="G317" s="15"/>
@@ -6617,7 +6498,7 @@
       <c r="C318" s="15"/>
       <c r="D318" s="16"/>
       <c r="E318" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F318" s="15"/>
       <c r="G318" s="15"/>
@@ -6630,7 +6511,7 @@
       <c r="C319" s="15"/>
       <c r="D319" s="16"/>
       <c r="E319" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F319" s="15"/>
       <c r="G319" s="15"/>
@@ -6643,7 +6524,7 @@
       <c r="C320" s="15"/>
       <c r="D320" s="16"/>
       <c r="E320" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F320" s="15"/>
       <c r="G320" s="15"/>
@@ -6656,7 +6537,7 @@
       <c r="C321" s="15"/>
       <c r="D321" s="16"/>
       <c r="E321" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F321" s="15"/>
       <c r="G321" s="15"/>
@@ -6669,7 +6550,7 @@
       <c r="C322" s="15"/>
       <c r="D322" s="16"/>
       <c r="E322" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F322" s="15"/>
       <c r="G322" s="15"/>

</xml_diff>